<commit_message>
Update: lemmatization-based cleaning; demo.py; README; correction map
</commit_message>
<xml_diff>
--- a/Test_output.xlsx
+++ b/Test_output.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>255339005</t>
+          <t>35489007</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>PROM - Premature rupture of membranes</t>
+          <t>Premature rupture of membranes</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Removal of tympanic ventilation tube from tympanic membrane (procedure)</t>
+          <t>Removal of tympanic ventilation tube from tympanic membrane</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Color Doppler ultrasound with spectral display for congenital anomaly (procedure)</t>
+          <t>Color Doppler ultrasound with spectral display for congenital anomaly</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Computed tomography of brain (procedure)</t>
+          <t>CT of brain</t>
         </is>
       </c>
     </row>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>255339005</t>
+          <t>35489007</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1315,12 +1315,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>251291004</t>
+          <t>738906000</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Dental measurement</t>
+          <t>Dental</t>
         </is>
       </c>
     </row>
@@ -1369,12 +1369,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>180301000119102</t>
+          <t>95677002</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>History of disorder of vision</t>
+          <t>Disorder of vision</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Plain X-ray of right foot (procedure)</t>
+          <t>Plain X-ray of right foot</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>16225231000119104</t>
+          <t>47639008</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1450,12 +1450,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>423736003</t>
+          <t>261197005</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Color Doppler flow</t>
+          <t>Doppler color flow</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Total hysterectomy with left oophorectomy (procedure)</t>
+          <t>Total hysterectomy with left oophorectomy</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Biopsy of cervical lymph node</t>
+          <t>Biopsy of cervical lymph node (procedure)</t>
         </is>
       </c>
     </row>
@@ -1612,12 +1612,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>11466000</t>
+          <t>161805006</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Cesarean section</t>
+          <t>History of cesarean section</t>
         </is>
       </c>
     </row>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>MRI of abdomen</t>
+          <t>Magnetic resonance imaging of abdomen</t>
         </is>
       </c>
     </row>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Vision screening (procedure)</t>
+          <t>Vision screening</t>
         </is>
       </c>
     </row>
@@ -1963,12 +1963,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>711554003</t>
+          <t>419553002</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Doppler ultrasound of pelvic vascular structure</t>
+          <t>US scan of pelvic vessels</t>
         </is>
       </c>
     </row>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>In vitro fertilization procedure</t>
+          <t>In vitro fertilization</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Screening for malignant neoplasm of cervix</t>
+          <t>Screening for malignant neoplasm of cervix (procedure)</t>
         </is>
       </c>
     </row>
@@ -2179,12 +2179,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>116762002</t>
+          <t>410652009</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Blood products administration</t>
+          <t>Blood product</t>
         </is>
       </c>
     </row>
@@ -2260,12 +2260,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>161653008</t>
+          <t>266719004</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>H/O: chemotherapy</t>
+          <t>Oral chemotherapy</t>
         </is>
       </c>
     </row>
@@ -2373,7 +2373,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Loop electrosurgical excision procedure (procedure)</t>
+          <t>Loop electrosurgical excision procedure</t>
         </is>
       </c>
     </row>
@@ -2503,12 +2503,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>396550006</t>
+          <t>87612001</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Blood test (procedure)</t>
+          <t>Blood</t>
         </is>
       </c>
     </row>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Biopsy of breast</t>
+          <t>Biopsy of breast (procedure)</t>
         </is>
       </c>
     </row>
@@ -2584,12 +2584,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>53281000</t>
+          <t>866149003</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Annual</t>
+          <t>Annual visit (procedure)</t>
         </is>
       </c>
     </row>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Circumcision</t>
+          <t>Circumcision (procedure)</t>
         </is>
       </c>
     </row>
@@ -2692,12 +2692,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>423736003</t>
+          <t>261197005</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Color Doppler flow</t>
+          <t>Doppler color flow</t>
         </is>
       </c>
     </row>
@@ -2746,12 +2746,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>396550006</t>
+          <t>87612001</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Blood test (procedure)</t>
+          <t>Blood</t>
         </is>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Digital tomosynthesis of breast</t>
+          <t>Digital breast tomosynthesis</t>
         </is>
       </c>
     </row>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Lead screening, blood (procedure)</t>
+          <t>Lead screening, blood</t>
         </is>
       </c>
     </row>
@@ -2962,12 +2962,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>300231003</t>
+          <t>127485006</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Remove object from mouth</t>
+          <t>Removes</t>
         </is>
       </c>
     </row>
@@ -3124,12 +3124,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>58059003</t>
+          <t>116863004</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Washing RBC for transfusion</t>
+          <t>Transfusion of red blood cells (procedure)</t>
         </is>
       </c>
     </row>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Anticardiolipin antibody measurement</t>
+          <t>Anticardiolipin antibody measurement (procedure)</t>
         </is>
       </c>
     </row>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Total bile acids measurement</t>
+          <t>Total bile acids measurement (procedure)</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Neutrophil count (procedure)</t>
+          <t>Neutrophil count</t>
         </is>
       </c>
     </row>
@@ -3421,12 +3421,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>81905004</t>
+          <t>250707004</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Globulin</t>
+          <t>Globulin measurement (procedure)</t>
         </is>
       </c>
     </row>
@@ -3745,12 +3745,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>165813002</t>
+          <t>250514000</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Human immunodeficiency virus antibody test</t>
+          <t>Human immunodeficiency virus antibody level</t>
         </is>
       </c>
     </row>
@@ -3799,12 +3799,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>167287002</t>
+          <t>167290008</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Urine ketones not detected</t>
+          <t>Urine ketone test = ++</t>
         </is>
       </c>
     </row>
@@ -3826,12 +3826,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>391374007</t>
+          <t>120646007</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>HSV IgM level</t>
+          <t>Antibody screen (procedure)</t>
         </is>
       </c>
     </row>
@@ -3912,7 +3912,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Urine microalbumin/creatinine ratio measurement (procedure)</t>
+          <t>Urine microalbumin/creatinine ratio measurement</t>
         </is>
       </c>
     </row>
@@ -3961,12 +3961,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>417389002</t>
+          <t>30061004</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Disorder of basophils</t>
+          <t>Basophil</t>
         </is>
       </c>
     </row>
@@ -4042,12 +4042,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>702675006</t>
+          <t>258066000</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>PCR</t>
+          <t>Polymerase chain reaction</t>
         </is>
       </c>
     </row>
@@ -4101,7 +4101,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Urine screening (procedure)</t>
+          <t>Urine screening</t>
         </is>
       </c>
     </row>
@@ -4150,12 +4150,12 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>401055007</t>
+          <t>271347000</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Self monitoring urine ketones (regime/therapy)</t>
+          <t>Urine ketone test</t>
         </is>
       </c>
     </row>
@@ -4204,12 +4204,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>275741008</t>
+          <t>52501007</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Leukocytes in urine</t>
+          <t>Leukocyte</t>
         </is>
       </c>
     </row>
@@ -4231,12 +4231,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>396550006</t>
+          <t>87612001</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Blood test (procedure)</t>
+          <t>Blood</t>
         </is>
       </c>
     </row>
@@ -4339,12 +4339,12 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>216750000</t>
+          <t>34957004</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Accidental poisoning by acids</t>
+          <t>Acid</t>
         </is>
       </c>
     </row>
@@ -4398,7 +4398,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Alpha fetoprotein</t>
+          <t>Alpha-fetoprotein</t>
         </is>
       </c>
     </row>
@@ -4420,12 +4420,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>17888004</t>
+          <t>9422000</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>HDL measurement</t>
+          <t>HDL</t>
         </is>
       </c>
     </row>
@@ -4447,12 +4447,12 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>415240008</t>
+          <t>118586006</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Ratio value</t>
+          <t>Ratios</t>
         </is>
       </c>
     </row>
@@ -4614,7 +4614,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Growth hormone measurement</t>
+          <t>Growth hormone measurement (procedure)</t>
         </is>
       </c>
     </row>
@@ -4636,12 +4636,12 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>416838001</t>
+          <t>365649001</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Erythrocyte sedimentation rate measurement (procedure)</t>
+          <t>Erythrocyte sedimentation rate</t>
         </is>
       </c>
     </row>
@@ -4717,12 +4717,12 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>117199004</t>
+          <t>64135003</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Islet cell antibody</t>
+          <t>Islet cell antibody measurement</t>
         </is>
       </c>
     </row>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Urobilinogen measurement, urine (procedure)</t>
+          <t>Urobilinogen measurement, urine</t>
         </is>
       </c>
     </row>
@@ -4830,7 +4830,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Immature reticulocyte fraction</t>
+          <t>Immature reticulocyte fraction (procedure)</t>
         </is>
       </c>
     </row>
@@ -4884,7 +4884,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Protein/creatinine ratio measurement</t>
+          <t>Protein/creatinine ratio measurement (procedure)</t>
         </is>
       </c>
     </row>
@@ -4906,12 +4906,12 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>269822005</t>
+          <t>71935002</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Hemoglobin A2 measurement</t>
+          <t>Hemoglobin A2</t>
         </is>
       </c>
     </row>
@@ -4992,7 +4992,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Urinalysis with reflex to microscopy</t>
+          <t>Urinalysis with reflex to microscopy (procedure)</t>
         </is>
       </c>
     </row>
@@ -5073,7 +5073,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Complete blood count without differential</t>
+          <t>Complete blood count without differential (procedure)</t>
         </is>
       </c>
     </row>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Urinalysis with reflex to microscopy</t>
+          <t>Urinalysis with reflex to microscopy (procedure)</t>
         </is>
       </c>
     </row>
@@ -5149,12 +5149,12 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>252282000</t>
+          <t>250346004</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Fibrinogen screening</t>
+          <t>Fibrinogen level</t>
         </is>
       </c>
     </row>
@@ -5257,12 +5257,12 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>314083002</t>
+          <t>312466004</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Urine opiates screening test</t>
+          <t>Urine opiate level</t>
         </is>
       </c>
     </row>
@@ -5424,7 +5424,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>White blood cell test (procedure)</t>
+          <t>White blood cell test</t>
         </is>
       </c>
     </row>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Urine pH test</t>
+          <t>Urine pH test (procedure)</t>
         </is>
       </c>
     </row>
@@ -5527,12 +5527,12 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>75828004</t>
+          <t>398137007</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Creatine kinase</t>
+          <t>Creatine kinase level</t>
         </is>
       </c>
     </row>
@@ -5559,7 +5559,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Fibrinogen titer (procedure)</t>
+          <t>Fibrinogen titer</t>
         </is>
       </c>
     </row>
@@ -5635,12 +5635,12 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>56136002</t>
+          <t>55918008</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Absolute</t>
+          <t>Monocyte</t>
         </is>
       </c>
     </row>
@@ -5662,12 +5662,12 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>18414002</t>
+          <t>448960003</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Vitamin D&gt;3&lt;</t>
+          <t>Injection of vitamin D</t>
         </is>
       </c>
     </row>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>Urine dipstick for specific gravity</t>
+          <t>Urine dipstick for specific gravity (procedure)</t>
         </is>
       </c>
     </row>
@@ -5797,12 +5797,12 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>121008006</t>
+          <t>121006005</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Influenza B virus Ag</t>
+          <t>Influenza A virus Ag</t>
         </is>
       </c>
     </row>
@@ -5932,12 +5932,12 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>399844005</t>
+          <t>277748003</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>FAST test</t>
+          <t>Fast</t>
         </is>
       </c>
     </row>
@@ -5986,12 +5986,12 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>275536003</t>
+          <t>14304000</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>History of thyroid disorder</t>
+          <t>Thyroid disorder</t>
         </is>
       </c>
     </row>
@@ -6040,12 +6040,12 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>313087008</t>
+          <t>405051006</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Anxiety counseling</t>
+          <t>Anxiety level</t>
         </is>
       </c>
     </row>
@@ -6472,12 +6472,12 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>396550006</t>
+          <t>49727002</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Blood test</t>
+          <t>Cough</t>
         </is>
       </c>
     </row>
@@ -6607,12 +6607,12 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>53148007</t>
+          <t>30760008</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Clubbing of toes</t>
+          <t>Finger clubbing</t>
         </is>
       </c>
     </row>
@@ -6688,12 +6688,12 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>402221000</t>
+          <t>238539001</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Acute-on-chronic vesicular eczema of hands</t>
+          <t>Hand eczema</t>
         </is>
       </c>
     </row>
@@ -6823,12 +6823,12 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>260378005</t>
+          <t>39928001</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Excessive</t>
+          <t>Excessive repair</t>
         </is>
       </c>
     </row>
@@ -7120,12 +7120,12 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>9499001</t>
+          <t>41329004</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>Multiple polyps</t>
+          <t>Polyp</t>
         </is>
       </c>
     </row>
@@ -7309,12 +7309,12 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>408760009</t>
+          <t>251776000</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Vision screening (procedure)</t>
+          <t>Ability to change between near and distance vision</t>
         </is>
       </c>
     </row>
@@ -7417,7 +7417,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>70819003</t>
+          <t>247441003</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
@@ -7471,12 +7471,12 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>268551005</t>
+          <t>161453001</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Obesity screening</t>
+          <t>History of obesity</t>
         </is>
       </c>
     </row>
@@ -7606,12 +7606,12 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>64572001</t>
+          <t>118935006</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Disorders</t>
+          <t>Disorder of hip</t>
         </is>
       </c>
     </row>
@@ -7687,12 +7687,12 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>40780007</t>
+          <t>86406008</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Human immunodeficiency virus I infection</t>
+          <t>Human immunodeficiency virus infection</t>
         </is>
       </c>
     </row>
@@ -7714,12 +7714,12 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>64572001</t>
+          <t>1010276004</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Disorders</t>
+          <t>Ring chromosome (disorder)</t>
         </is>
       </c>
     </row>
@@ -7768,12 +7768,12 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>267038008</t>
+          <t>278804003</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Edema</t>
+          <t>Lees screening</t>
         </is>
       </c>
     </row>
@@ -7849,12 +7849,12 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>408442008</t>
+          <t>90935002</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Hemophilia</t>
+          <t>Hemophilia (disorder)</t>
         </is>
       </c>
     </row>
@@ -7876,12 +7876,12 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>199112006</t>
+          <t>302812006</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Infections of the genital tract in pregnancy</t>
+          <t>Anogenital human papillomavirus infection</t>
         </is>
       </c>
     </row>
@@ -7903,7 +7903,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>267038008</t>
+          <t>79654002</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -7984,12 +7984,12 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>715799004</t>
+          <t>719980006</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Charcot-Marie-Tooth disease type 4G</t>
+          <t>Charcot-Marie-Tooth disease type IF</t>
         </is>
       </c>
     </row>
@@ -8097,7 +8097,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>History of osteoarthritis</t>
+          <t>H/O: osteoarthritis</t>
         </is>
       </c>
     </row>
@@ -8119,12 +8119,12 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>35240004</t>
+          <t>171198002</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Iron deficiency</t>
+          <t>Iron deficiency screening (procedure)</t>
         </is>
       </c>
     </row>
@@ -8173,12 +8173,12 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>371240000</t>
+          <t>118708007</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Procedure on hand</t>
         </is>
       </c>
     </row>
@@ -8281,12 +8281,12 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>1304272004</t>
+          <t>102573001</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Edema of bilateral thighs</t>
+          <t>Edema of thigh</t>
         </is>
       </c>
     </row>
@@ -8362,12 +8362,12 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>13492002</t>
+          <t>39840002</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Blood group antibody Di^b^</t>
+          <t>Blood group antibody Di^a^</t>
         </is>
       </c>
     </row>
@@ -8605,12 +8605,12 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>2371960</t>
+          <t>11253</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>vitamin E 6.75 MG</t>
+          <t>vitamin D</t>
         </is>
       </c>
     </row>
@@ -8632,12 +8632,12 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>1649405</t>
+          <t>1791505</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>doxycycline hyclate 50 MG Oral Capsule</t>
+          <t>doxycycline hyclate 75 MG Oral Capsule</t>
         </is>
       </c>
     </row>
@@ -8875,12 +8875,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>311486</t>
+          <t>152695</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>meloxicam 7.5 MG Oral Tablet</t>
+          <t>meloxicam 15 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -8902,12 +8902,12 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>1247759</t>
+          <t>1248224</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>docusate sodium 50 MG Oral Capsule</t>
+          <t>docusate sodium 200 MG Oral Capsule</t>
         </is>
       </c>
     </row>
@@ -8929,12 +8929,12 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>198405</t>
+          <t>197806</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>ibuprofen 100 MG Oral Tablet</t>
+          <t>ibuprofen 600 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -8956,12 +8956,12 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>1807630</t>
+          <t>1807636</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>sodium chloride 0.9 % per 25 ML Injection</t>
+          <t>sodium chloride 0.9 % per 2 ML Injection</t>
         </is>
       </c>
     </row>
@@ -9091,12 +9091,12 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>199079</t>
+          <t>430835</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>acetaminophen 80 MG Oral Tablet</t>
+          <t>acetaminophen 250 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -9118,12 +9118,12 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>370576</t>
+          <t>105151</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>amoxicillin Oral Suspension</t>
+          <t>amoxicillin 750 MG Oral Suspension</t>
         </is>
       </c>
     </row>
@@ -9145,12 +9145,12 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>152855</t>
+          <t>151227</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Topamax 25 MG Oral Tablet</t>
+          <t>Topamax 50 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -9253,12 +9253,12 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>152855</t>
+          <t>151227</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Topamax 25 MG Oral Tablet</t>
+          <t>Topamax 50 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -9361,12 +9361,12 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>242891</t>
+          <t>242892</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>estradiol 0.05 MG/Day Twice Weekly Transdermal System</t>
+          <t>estradiol 0.1 MG/Day Twice Weekly Transdermal System</t>
         </is>
       </c>
     </row>
@@ -9388,12 +9388,12 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>849517</t>
+          <t>430835</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>DDAVP Tablets 0.1 MG Oral Tablet</t>
+          <t>acetaminophen 250 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -9442,12 +9442,12 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>2563975</t>
+          <t>2658591</t>
         </is>
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>insulin glargine-yfgn 100 UNT/ML Pen Injector [Semglee]</t>
+          <t>insulin glargine-yfgn Pen Injector [Semglee]</t>
         </is>
       </c>
     </row>
@@ -9496,12 +9496,12 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>1359855</t>
+          <t>847230</t>
         </is>
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>insulin glargine 100 UNT/ML Pen Injector</t>
+          <t>3 ML insulin glargine 100 UNT/ML Pen Injector</t>
         </is>
       </c>
     </row>
@@ -9550,12 +9550,12 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>544391</t>
+          <t>854761</t>
         </is>
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>ibuprofen 20 MG/ML [Motrin]</t>
+          <t>ibuprofen 40 MG/ML [Motrin]</t>
         </is>
       </c>
     </row>
@@ -9604,12 +9604,12 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>544393</t>
+          <t>854762</t>
         </is>
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Motrin 20 MG/ML Oral Suspension</t>
+          <t>Motrin 40 MG/ML Oral Suspension</t>
         </is>
       </c>
     </row>
@@ -9631,12 +9631,12 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>333210</t>
+          <t>333209</t>
         </is>
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>prednisolone 25 MG</t>
+          <t>prednisolone 1 MG</t>
         </is>
       </c>
     </row>
@@ -9712,12 +9712,12 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>896013</t>
+          <t>896001</t>
         </is>
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Flovent HFA 220 MCG/ACTUAT Metered Dose Inhaler, 60 ACTUAT</t>
+          <t>Flovent HFA 110 MCG/INHAL Metered Dose Inhaler, 120 Actuations</t>
         </is>
       </c>
     </row>
@@ -9820,12 +9820,12 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>389242</t>
+          <t>135805</t>
         </is>
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>deferiprone 500 MG Three-Times-A-Day Oral Tablet</t>
+          <t>Humalog</t>
         </is>
       </c>
     </row>
@@ -9901,12 +9901,12 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>329760</t>
+          <t>334770</t>
         </is>
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>ferrous sulfate 325 MG</t>
+          <t>ferrous sulfate 160 MG</t>
         </is>
       </c>
     </row>
@@ -9987,7 +9987,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Estrace 0.01 % Vaginal Cream</t>
+          <t>ESTRACE 0.01 % Vaginal Cream</t>
         </is>
       </c>
     </row>
@@ -10063,12 +10063,12 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>745277</t>
+          <t>745279</t>
         </is>
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>penicillin G potassium 313 MG</t>
+          <t>penicillin G potassium 125 MG</t>
         </is>
       </c>
     </row>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>diphenhydramine Oral Tablet [Benadryl]</t>
+          <t>diphenhydrAMINE Oral Tablet [Benadryl]</t>
         </is>
       </c>
     </row>
@@ -10117,12 +10117,12 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>1807630</t>
+          <t>1807636</t>
         </is>
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>sodium chloride 0.9 % per 25 ML Injection</t>
+          <t>sodium chloride 0.9 % per 2 ML Injection</t>
         </is>
       </c>
     </row>
@@ -10171,12 +10171,12 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>1870358</t>
+          <t>876193</t>
         </is>
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>polyethylene glycol 3350 Powder for Oral Solution</t>
+          <t>polyethylene glycol 3350 17000 MG Powder for Oral Solution</t>
         </is>
       </c>
     </row>
@@ -10225,12 +10225,12 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>437233</t>
+          <t>336365</t>
         </is>
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>acetaminophen 330 MG</t>
+          <t>acetaminophen 25 MG</t>
         </is>
       </c>
     </row>
@@ -10495,12 +10495,12 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>1545668</t>
+          <t>1545664</t>
         </is>
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>Jardiance 25 MG Oral Tablet</t>
+          <t>Jardiance 10 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -10522,12 +10522,12 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>1359856</t>
+          <t>847232</t>
         </is>
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>insulin glargine 100 UNT/ML Pen Injector [Lantus]</t>
+          <t>3 ML insulin glargine 100 UNT/ML Pen Injector [Lantus]</t>
         </is>
       </c>
     </row>
@@ -10549,12 +10549,12 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>1608797</t>
+          <t>849431</t>
         </is>
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>naproxen 200 MG Oral Tablet</t>
+          <t>naproxen sodium 550 MG (as naproxen 500 MG) Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -10603,12 +10603,12 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>1998774</t>
+          <t>1998772</t>
         </is>
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>QVAR Redihaler 40 MCG/ACTUAT Breath-Actuated Metered Dose Inhaler, 120 ACTUAT</t>
+          <t>QVAR Redihaler 80 MCG/ACTUAT Breath-Actuated Metered Dose Inhaler, 120 ACTUAT</t>
         </is>
       </c>
     </row>
@@ -10657,12 +10657,12 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>2648708</t>
+          <t>1941605</t>
         </is>
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>fluticasone propionate Metered Dose Nasal Spray</t>
+          <t>fluticasone propionate 232 MCG/INHAL Dry Powder Inhaler, 60 Actuations</t>
         </is>
       </c>
     </row>
@@ -10819,12 +10819,12 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>198405</t>
+          <t>197806</t>
         </is>
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>ibuprofen 100 MG Oral Tablet</t>
+          <t>ibuprofen 600 MG Oral Tablet</t>
         </is>
       </c>
     </row>
@@ -11040,7 +11040,7 @@
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>Rotarix, Rotavirus, live attenuated (RV1) G1P[8] Vaccine 1.5 mL Oral Suspension</t>
+          <t>Rotarix, Rotavirus, live attenuated (RV1) G1P[8] Vaccine 1.5 ML Oral Suspension</t>
         </is>
       </c>
     </row>
@@ -11116,12 +11116,12 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>438507</t>
+          <t>316256</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>metformin 513 MG</t>
+          <t>metFORMIN 500 MG</t>
         </is>
       </c>
     </row>
@@ -11256,7 +11256,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>diphenhydramine</t>
+          <t>diphenhydrAMINE</t>
         </is>
       </c>
     </row>

</xml_diff>